<commit_message>
running remainder ants; moving sessions & analyses to project
</commit_message>
<xml_diff>
--- a/code/validation_sessions_2021.11.16_WT.xlsx
+++ b/code/validation_sessions_2021.11.16_WT.xlsx
@@ -303,8 +303,8 @@
   </sheetPr>
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K50" activeCellId="0" sqref="K50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L27" activeCellId="0" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -312,7 +312,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="48.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="65.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="23.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.06"/>
   </cols>

</xml_diff>